<commit_message>
Change the control of each of the system metadata fields, where essentially the MN controls all fields except for the replica entries.
</commit_message>
<xml_diff>
--- a/source/design/data/SysMetaMutability.xlsx
+++ b/source/design/data/SysMetaMutability.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="25260" yWindow="7980" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="46">
   <si>
     <t>Property</t>
   </si>
@@ -108,15 +108,9 @@
     <t>client</t>
   </si>
   <si>
-    <t>CNAuthorization.setOwner</t>
-  </si>
-  <si>
     <t>rightsHolder, CN Administrator</t>
   </si>
   <si>
-    <t>CNAuthorization.setAccessPolicy, MNStorage.update (calls CN setAccessPolicy)</t>
-  </si>
-  <si>
     <t>subjects with changePermission permission</t>
   </si>
   <si>
@@ -126,28 +120,43 @@
     <t>subjects with write permission</t>
   </si>
   <si>
-    <t>MNStorage.update</t>
-  </si>
-  <si>
-    <t>MNStorage.delete</t>
-  </si>
-  <si>
     <t>Various - any change to system metadata</t>
   </si>
   <si>
     <t>Manual update process</t>
   </si>
   <si>
-    <t>Someone with access to CNs</t>
-  </si>
-  <si>
-    <t>CNReplication.updateReplicationMetadata</t>
-  </si>
-  <si>
     <t>ModifiableBy</t>
   </si>
   <si>
     <t>Various</t>
+  </si>
+  <si>
+    <t>CNReplication.updateReplicationMetadata()</t>
+  </si>
+  <si>
+    <t>MN/CN</t>
+  </si>
+  <si>
+    <t>Someone with access to MNs/CNs</t>
+  </si>
+  <si>
+    <t>MNCore.archive()</t>
+  </si>
+  <si>
+    <t>MNStorage.update()</t>
+  </si>
+  <si>
+    <t>MNCore.setObsoletedBy(), MNStorage.update()</t>
+  </si>
+  <si>
+    <t>manual (Tier 1), MNAuthorization.setAccessPolicy(), MNStorage.update ()(all must call CNAuthorization.systemMetadataChanged())</t>
+  </si>
+  <si>
+    <t>MNAuthorization.setRightsHolder()</t>
+  </si>
+  <si>
+    <t>MN-service-subject</t>
   </si>
 </sst>
 </file>
@@ -558,7 +567,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -589,7 +598,7 @@
         <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -601,16 +610,16 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -697,13 +706,13 @@
         <v>19</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30">
+    </row>
+    <row r="9" spans="1:7" ht="45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -717,10 +726,10 @@
         <v>19</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -737,10 +746,10 @@
         <v>19</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -757,10 +766,10 @@
         <v>19</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -777,10 +786,10 @@
         <v>19</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -797,10 +806,10 @@
         <v>19</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -825,13 +834,13 @@
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
         <v>19</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -842,7 +851,7 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
         <v>21</v>
@@ -856,13 +865,13 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F17" t="s">
         <v>39</v>
@@ -882,7 +891,7 @@
         <v>19</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F18" t="s">
         <v>25</v>
@@ -890,7 +899,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Modified mutability chart to indicate that format should be mutable in future versions of system metadata policies.
</commit_message>
<xml_diff>
--- a/source/design/data/SysMetaMutability.xlsx
+++ b/source/design/data/SysMetaMutability.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25260" yWindow="7980" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -567,7 +567,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -647,7 +647,7 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7">

</xml_diff>

<commit_message>
Update the table to reflect changes in the roadmap proposal.  Basically just CNAuth.systemMetadataChanged() --> CNCore.systemMetadataChanged() .
</commit_message>
<xml_diff>
--- a/source/design/data/SysMetaMutability.xlsx
+++ b/source/design/data/SysMetaMutability.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
@@ -114,9 +114,6 @@
     <t>subjects with changePermission permission</t>
   </si>
   <si>
-    <t>CNReplication.setReplicationPolicy</t>
-  </si>
-  <si>
     <t>subjects with write permission</t>
   </si>
   <si>
@@ -150,13 +147,16 @@
     <t>MNCore.setObsoletedBy(), MNStorage.update()</t>
   </si>
   <si>
-    <t>manual (Tier 1), MNAuthorization.setAccessPolicy(), MNStorage.update ()(all must call CNAuthorization.systemMetadataChanged())</t>
-  </si>
-  <si>
     <t>MNAuthorization.setRightsHolder()</t>
   </si>
   <si>
     <t>MN-service-subject</t>
+  </si>
+  <si>
+    <t>CNReplication.setReplicationPolicy()</t>
+  </si>
+  <si>
+    <t>manual (Tier 1), MNAuthorization.setAccessPolicy(), MNStorage.update ()(all must call CNCore.systemMetadataChanged())</t>
   </si>
 </sst>
 </file>
@@ -567,7 +567,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -598,7 +598,7 @@
         <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -616,10 +616,10 @@
         <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -706,7 +706,7 @@
         <v>19</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F8" t="s">
         <v>29</v>
@@ -726,7 +726,7 @@
         <v>19</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F9" t="s">
         <v>30</v>
@@ -746,10 +746,10 @@
         <v>19</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
         <v>31</v>
-      </c>
-      <c r="F10" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -766,10 +766,10 @@
         <v>19</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -786,10 +786,10 @@
         <v>19</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -806,10 +806,10 @@
         <v>19</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -840,7 +840,7 @@
         <v>19</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -865,16 +865,16 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" t="s">
         <v>38</v>
-      </c>
-      <c r="D17" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -891,7 +891,7 @@
         <v>19</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F18" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
change serialVersion to be managed by the CN replication processes. https://redmine.dataone.org/issues/3729
</commit_message>
<xml_diff>
--- a/source/design/data/SysMetaMutability.xlsx
+++ b/source/design/data/SysMetaMutability.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
@@ -150,13 +150,13 @@
     <t>MNAuthorization.setRightsHolder()</t>
   </si>
   <si>
-    <t>MN-service-subject</t>
-  </si>
-  <si>
     <t>CNReplication.setReplicationPolicy()</t>
   </si>
   <si>
     <t>manual (Tier 1), MNAuthorization.setAccessPolicy(), MNStorage.update ()(all must call CNCore.systemMetadataChanged())</t>
+  </si>
+  <si>
+    <t>CN replication processes</t>
   </si>
 </sst>
 </file>
@@ -567,7 +567,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -610,7 +610,7 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -619,7 +619,7 @@
         <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -726,7 +726,7 @@
         <v>19</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F9" t="s">
         <v>30</v>
@@ -746,7 +746,7 @@
         <v>19</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Add the mutability about seriesId.
</commit_message>
<xml_diff>
--- a/source/design/data/SysMetaMutability.xlsx
+++ b/source/design/data/SysMetaMutability.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="11180" yWindow="3240" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="47">
   <si>
     <t>Property</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>CN replication processes</t>
+  </si>
+  <si>
+    <t>seriesId</t>
   </si>
 </sst>
 </file>
@@ -564,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -897,6 +900,20 @@
         <v>25</v>
       </c>
     </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>